<commit_message>
made basic unlockable bundle textures; moved intro quest to Krobus events file and updated for 1.6; removed quest framework dependency; added unlockable bundles dependency; moved quest board to side on map to make room for collection basket
</commit_message>
<xml_diff>
--- a/[Si] Lair of Shadows/[CP] Lair of Shadows/Chars.xlsx
+++ b/[Si] Lair of Shadows/[CP] Lair of Shadows/Chars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Steam\Steam\steamapps\common\Stardew Valley\SiMods\[Si]\.Projects\.ShadowSanctuary\[Si] Lair of Shadows\[CP] Lair of Shadows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D894B5CC-E4BE-4150-81FD-DCB23A44AC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF81560-358C-42B4-9776-116318E3F197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="101">
   <si>
     <t>Fetta</t>
   </si>
@@ -325,6 +325,21 @@
   </si>
   <si>
     <t>Tove</t>
+  </si>
+  <si>
+    <t>New ID</t>
+  </si>
+  <si>
+    <t>Intro1</t>
+  </si>
+  <si>
+    <t>Intro2</t>
+  </si>
+  <si>
+    <t>Intro3</t>
+  </si>
+  <si>
+    <t>Intro4</t>
   </si>
 </sst>
 </file>
@@ -1136,1137 +1151,1153 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A12419-1E06-4537-9746-97A990338324}">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="3" width="9.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="2"/>
-    <col min="5" max="5" width="0.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="1" max="2" width="11.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="9.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="2"/>
+    <col min="6" max="6" width="0.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>262205000</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>262205001</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>262205002</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>262205003</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>262205004</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>262205005</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>262205006</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>262205007</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>262205008</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>262205009</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="E11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>262205010</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="E12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>262205011</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="E13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>262205012</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="E14" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>262205013</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="E15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>262205014</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="E16" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>262205015</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>262205016</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="E18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>262205017</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="E19" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>262205018</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="E20" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>262205019</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="E21" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>262205020</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7">
         <v>262205021</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>31</v>
-      </c>
+      <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="E23" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="7"/>
+      <c r="G23" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="H23" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>262205022</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="F24" t="s">
+      <c r="E24" s="9"/>
+      <c r="G24" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>262205023</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="G25" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>262205024</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="F26" t="s">
+      <c r="E26" s="9"/>
+      <c r="G26" t="s">
         <v>66</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>262205025</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>262205026</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="G28" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>262205027</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="9"/>
-      <c r="F29" t="s">
+      <c r="E29" s="9"/>
+      <c r="G29" t="s">
         <v>66</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>262205028</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>30</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="H30" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>262205029</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="G31" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>262205030</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="G32" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>262205031</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C33" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="9"/>
-      <c r="F33" t="s">
+      <c r="E33" s="9"/>
+      <c r="G33" t="s">
         <v>66</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>262205032</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="G34" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>262205033</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C35" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="9"/>
-      <c r="F35" t="s">
+      <c r="E35" s="9"/>
+      <c r="G35" t="s">
         <v>66</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>262205034</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>262205035</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>262205036</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C38" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="F38" t="s">
+      <c r="E38" s="9"/>
+      <c r="G38" t="s">
         <v>66</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>262205037</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C39" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="G39" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>262205038</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C40" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="9"/>
-      <c r="F40" t="s">
+      <c r="E40" s="9"/>
+      <c r="G40" t="s">
         <v>66</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="H40" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>262205039</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C41" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="9"/>
-      <c r="F41" t="s">
+      <c r="E41" s="9"/>
+      <c r="G41" t="s">
         <v>66</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="H41" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>262205040</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C42" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="G42" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>262205041</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C43" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>262205042</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C44" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>262205043</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C45" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>262205044</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C46" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="G46" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>262205045</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>262205046</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>262205047</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C49" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="9"/>
-      <c r="F49" t="s">
+      <c r="E49" s="9"/>
+      <c r="G49" t="s">
         <v>66</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>262205048</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C50" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="G50" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>262205049</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>262205050</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>262205051</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C53" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="G53" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>262205052</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C54" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F54" s="11" t="s">
+      <c r="G54" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>262205053</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C55" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D55" s="9"/>
-      <c r="F55" t="s">
+      <c r="E55" s="9"/>
+      <c r="G55" t="s">
         <v>66</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="H55" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>262205054</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C56" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D56" s="9"/>
-      <c r="F56" t="s">
+      <c r="E56" s="9"/>
+      <c r="G56" t="s">
         <v>66</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="H56" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>262205055</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C57" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D57" s="10" t="s">
+      <c r="E57" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F57" s="11" t="s">
+      <c r="G57" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>262205056</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C58" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D58" s="9"/>
-      <c r="F58" t="s">
+      <c r="E58" s="9"/>
+      <c r="G58" t="s">
         <v>66</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="H58" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>262205057</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>262205058</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F60" t="s">
+      <c r="G60" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>262205059</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C61" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D61" s="9"/>
-      <c r="F61" t="s">
+      <c r="E61" s="9"/>
+      <c r="G61" t="s">
         <v>66</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="H61" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>262205060</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C62" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F62" s="11" t="s">
+      <c r="G62" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>262205061</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C63" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
         <v>66</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="H63" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>262205062</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="D64" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G64" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>262205063</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="D65" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G65" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>262205064</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C66" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F66" t="s">
+        <v>31</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G66" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>262205065</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C67" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F67" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G67" s="11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>262205066</v>
       </c>
-      <c r="F68" t="s">
+      <c r="G68" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>262205067</v>
       </c>
-      <c r="F69" t="s">
+      <c r="G69" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>262205068</v>
       </c>
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>262205069</v>
       </c>
-      <c r="F71" t="s">
+      <c r="G71" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="7">
         <v>262205070</v>
       </c>
@@ -2274,21 +2305,22 @@
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
-      <c r="F72" s="8" t="s">
+      <c r="F72" s="7"/>
+      <c r="G72" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>262205071</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C73" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F73" t="s">
+      <c r="G73" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed first bundle icon name, updated tracking sheet, tweaked intor questline; ready for testing
</commit_message>
<xml_diff>
--- a/[Si] Lair of Shadows/[CP] Lair of Shadows/Chars.xlsx
+++ b/[Si] Lair of Shadows/[CP] Lair of Shadows/Chars.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Steam\Steam\steamapps\common\Stardew Valley\SiMods\[Si]\.Projects\.ShadowSanctuary\[Si] Lair of Shadows\[CP] Lair of Shadows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Steam\Steam\steamapps\common\Stardew Valley\SiMods\[Si]\.WIP\ShadowSanctuary\[Si] Lair of Shadows\[CP] Lair of Shadows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF81560-358C-42B4-9776-116318E3F197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF737E17-3DF4-4562-A17B-E4B679B63ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="117">
   <si>
     <t>Fetta</t>
   </si>
@@ -153,24 +153,6 @@
     <t>Fly quest</t>
   </si>
   <si>
-    <t>Fly quest noletter</t>
-  </si>
-  <si>
-    <t>Event gives clay and bone quests</t>
-  </si>
-  <si>
-    <t>Clay quest</t>
-  </si>
-  <si>
-    <t>Bone quest</t>
-  </si>
-  <si>
-    <t>Bone quest noletter</t>
-  </si>
-  <si>
-    <t>Clay quest noletter</t>
-  </si>
-  <si>
     <t>Event gives wiz and guild quests</t>
   </si>
   <si>
@@ -186,9 +168,6 @@
     <t>Guild gives slay monsters quest</t>
   </si>
   <si>
-    <t>Slay monsters quest noletter</t>
-  </si>
-  <si>
     <t>Return to guild</t>
   </si>
   <si>
@@ -198,9 +177,6 @@
     <t>Totem quest</t>
   </si>
   <si>
-    <t>Totem quest noletter</t>
-  </si>
-  <si>
     <t>Event gives mine quest</t>
   </si>
   <si>
@@ -340,13 +316,85 @@
   </si>
   <si>
     <t>Intro4</t>
+  </si>
+  <si>
+    <t>Intro event, strange bun quest</t>
+  </si>
+  <si>
+    <t>Fly quest done</t>
+  </si>
+  <si>
+    <t>Event gives clay and bone bundke</t>
+  </si>
+  <si>
+    <t>Clay and bone bundle</t>
+  </si>
+  <si>
+    <t>Clay and bone bundle done</t>
+  </si>
+  <si>
+    <t>Intro5</t>
+  </si>
+  <si>
+    <t>Intro6</t>
+  </si>
+  <si>
+    <t>Intro7</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Intro8</t>
+  </si>
+  <si>
+    <t>Intro9</t>
+  </si>
+  <si>
+    <t>Intro10</t>
+  </si>
+  <si>
+    <t>Intro11</t>
+  </si>
+  <si>
+    <t>Intro12</t>
+  </si>
+  <si>
+    <t>Totem quest done</t>
+  </si>
+  <si>
+    <t>Intro13</t>
+  </si>
+  <si>
+    <t>Intro14</t>
+  </si>
+  <si>
+    <t>Intro15</t>
+  </si>
+  <si>
+    <t>Slay monsters quest done</t>
+  </si>
+  <si>
+    <t>Intro16</t>
+  </si>
+  <si>
+    <t>Intro17</t>
+  </si>
+  <si>
+    <t>Intro18</t>
+  </si>
+  <si>
+    <t>Intro19</t>
+  </si>
+  <si>
+    <t>Intro20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +406,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -726,7 +780,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1154,12 +1208,13 @@
   <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="2"/>
     <col min="4" max="4" width="9.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="2"/>
@@ -1172,7 +1227,7 @@
         <v>25</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>26</v>
@@ -1193,7 +1248,7 @@
         <v>262205000</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>31</v>
@@ -1205,7 +1260,7 @@
         <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1213,7 +1268,7 @@
         <v>262205001</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>31</v>
@@ -1233,7 +1288,7 @@
         <v>262205002</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>32</v>
@@ -1253,7 +1308,7 @@
         <v>262205003</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -1265,13 +1320,16 @@
         <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>262205004</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>31</v>
       </c>
@@ -1282,13 +1340,16 @@
         <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>262205005</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>32</v>
       </c>
@@ -1299,13 +1360,16 @@
         <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>262205006</v>
       </c>
+      <c r="B8" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
@@ -1316,13 +1380,16 @@
         <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>262205007</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
@@ -1331,15 +1398,15 @@
       </c>
       <c r="E9" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="G9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>262205008</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="C10" s="2" t="s">
         <v>33</v>
       </c>
@@ -1348,15 +1415,15 @@
       </c>
       <c r="E10" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="G10" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>262205009</v>
       </c>
+      <c r="B11" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>31</v>
       </c>
@@ -1367,13 +1434,16 @@
         <v>35</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>262205010</v>
       </c>
+      <c r="B12" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>32</v>
       </c>
@@ -1384,13 +1454,16 @@
         <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>262205011</v>
       </c>
+      <c r="B13" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
@@ -1401,13 +1474,16 @@
         <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>262205012</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>31</v>
       </c>
@@ -1418,66 +1494,78 @@
         <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>262205013</v>
       </c>
+      <c r="B15" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="C15" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>35</v>
+      <c r="E15" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>262205014</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="C16" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>35</v>
+      <c r="E16" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="G16" t="s">
-        <v>49</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>262205015</v>
       </c>
+      <c r="B17" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="10" t="s">
-        <v>34</v>
+      <c r="E17" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="G17" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>262205016</v>
       </c>
+      <c r="B18" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="C18" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>29</v>
@@ -1486,32 +1574,38 @@
         <v>35</v>
       </c>
       <c r="G18" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>262205017</v>
       </c>
+      <c r="B19" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="C19" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>34</v>
+      <c r="E19" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="G19" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>262205018</v>
       </c>
+      <c r="B20" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="C20" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>29</v>
@@ -1520,13 +1614,16 @@
         <v>34</v>
       </c>
       <c r="G20" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>262205019</v>
       </c>
+      <c r="B21" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="C21" s="2" t="s">
         <v>31</v>
       </c>
@@ -1537,13 +1634,16 @@
         <v>34</v>
       </c>
       <c r="G21" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>262205020</v>
       </c>
+      <c r="B22" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>32</v>
       </c>
@@ -1554,14 +1654,16 @@
         <v>34</v>
       </c>
       <c r="G22" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7">
         <v>262205021</v>
       </c>
-      <c r="B23" s="7"/>
+      <c r="B23" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="C23" s="7" t="s">
         <v>31</v>
       </c>
@@ -1573,10 +1675,10 @@
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="8" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1591,10 +1693,10 @@
       </c>
       <c r="E24" s="9"/>
       <c r="G24" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1623,10 +1725,10 @@
       </c>
       <c r="E26" s="9"/>
       <c r="G26" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1643,7 +1745,7 @@
         <v>30</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1660,7 +1762,7 @@
         <v>30</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -1675,10 +1777,10 @@
       </c>
       <c r="E29" s="9"/>
       <c r="G29" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -1695,7 +1797,7 @@
         <v>30</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -1712,7 +1814,7 @@
         <v>30</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -1723,10 +1825,10 @@
         <v>31</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -1737,14 +1839,14 @@
         <v>31</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E33" s="9"/>
       <c r="G33" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -1755,7 +1857,7 @@
         <v>31</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G34" s="11" t="s">
         <v>30</v>
@@ -1769,14 +1871,14 @@
         <v>31</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E35" s="9"/>
       <c r="G35" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -1787,10 +1889,10 @@
         <v>32</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G36" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -1801,10 +1903,10 @@
         <v>33</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G37" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -1815,14 +1917,14 @@
         <v>31</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E38" s="9"/>
       <c r="G38" t="s">
+        <v>58</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -1833,7 +1935,7 @@
         <v>31</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G39" s="11" t="s">
         <v>30</v>
@@ -1851,10 +1953,10 @@
       </c>
       <c r="E40" s="9"/>
       <c r="G40" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -1869,10 +1971,10 @@
       </c>
       <c r="E41" s="9"/>
       <c r="G41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -1897,10 +1999,10 @@
         <v>31</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G43" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -1911,10 +2013,10 @@
         <v>31</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G44" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -1925,10 +2027,10 @@
         <v>31</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G45" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -1939,10 +2041,10 @@
         <v>31</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -1956,7 +2058,7 @@
         <v>7</v>
       </c>
       <c r="G47" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -1970,7 +2072,7 @@
         <v>7</v>
       </c>
       <c r="G48" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
@@ -1985,10 +2087,10 @@
       </c>
       <c r="E49" s="9"/>
       <c r="G49" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -2016,7 +2118,7 @@
         <v>8</v>
       </c>
       <c r="G51" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -2030,7 +2132,7 @@
         <v>8</v>
       </c>
       <c r="G52" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -2055,10 +2157,10 @@
         <v>31</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G54" s="11" t="s">
         <v>57</v>
-      </c>
-      <c r="G54" s="11" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
@@ -2073,10 +2175,10 @@
       </c>
       <c r="E55" s="9"/>
       <c r="G55" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -2091,10 +2193,10 @@
       </c>
       <c r="E56" s="9"/>
       <c r="G56" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -2122,14 +2224,14 @@
         <v>31</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E58" s="9"/>
       <c r="G58" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
@@ -2140,10 +2242,10 @@
         <v>32</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G59" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
@@ -2154,10 +2256,10 @@
         <v>33</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G60" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
@@ -2168,14 +2270,14 @@
         <v>31</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E61" s="9"/>
       <c r="G61" t="s">
+        <v>58</v>
+      </c>
+      <c r="H61" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
@@ -2186,7 +2288,7 @@
         <v>31</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G62" s="11" t="s">
         <v>30</v>
@@ -2203,10 +2305,10 @@
         <v>1</v>
       </c>
       <c r="G63" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
@@ -2220,7 +2322,7 @@
         <v>1</v>
       </c>
       <c r="G64" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -2234,7 +2336,7 @@
         <v>1</v>
       </c>
       <c r="G65" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2248,7 +2350,7 @@
         <v>1</v>
       </c>
       <c r="G66" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -2262,7 +2364,7 @@
         <v>1</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -2270,7 +2372,7 @@
         <v>262205066</v>
       </c>
       <c r="G68" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -2278,7 +2380,7 @@
         <v>262205067</v>
       </c>
       <c r="G69" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -2286,7 +2388,7 @@
         <v>262205068</v>
       </c>
       <c r="G70" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -2294,7 +2396,7 @@
         <v>262205069</v>
       </c>
       <c r="G71" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:7" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2307,7 +2409,7 @@
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
       <c r="G72" s="8" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -2321,10 +2423,11 @@
         <v>29</v>
       </c>
       <c r="G73" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Tweaking and testing intro questline and main map; making my peace with the bugs for now
</commit_message>
<xml_diff>
--- a/[Si] Lair of Shadows/[CP] Lair of Shadows/Chars.xlsx
+++ b/[Si] Lair of Shadows/[CP] Lair of Shadows/Chars.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Steam\Steam\steamapps\common\Stardew Valley\SiMods\[Si]\.WIP\ShadowSanctuary\[Si] Lair of Shadows\[CP] Lair of Shadows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Steam\Steam\steamapps\common\Stardew Valley\SiMods\[Si]\ShadowSanctuary\[Si] Lair of Shadows\[CP] Lair of Shadows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2E13A0-4B31-48B3-8053-5C79B805BEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46FDDDD-3989-4854-AE74-2955D4AA2A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="129">
   <si>
     <t>Bellum</t>
   </si>
@@ -177,12 +177,6 @@
     <t>Intro event, strange bun quest</t>
   </si>
   <si>
-    <t>Fly quest done</t>
-  </si>
-  <si>
-    <t>Event gives clay and bone bundke</t>
-  </si>
-  <si>
     <t>Clay and bone bundle</t>
   </si>
   <si>
@@ -400,6 +394,36 @@
   </si>
   <si>
     <t>Glee1</t>
+  </si>
+  <si>
+    <t>Intro3b</t>
+  </si>
+  <si>
+    <t>Trigger</t>
+  </si>
+  <si>
+    <t>Fly quest done trigger action</t>
+  </si>
+  <si>
+    <t>Fly quest done letter</t>
+  </si>
+  <si>
+    <t>Letter</t>
+  </si>
+  <si>
+    <t>Event gives clay and bone bundle</t>
+  </si>
+  <si>
+    <t>Intro15b</t>
+  </si>
+  <si>
+    <t>Return to guild quest</t>
+  </si>
+  <si>
+    <t>Intro15c</t>
+  </si>
+  <si>
+    <t>Monster quest done trigger action</t>
   </si>
 </sst>
 </file>
@@ -792,16 +816,16 @@
         <v>10</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>11</v>
@@ -821,7 +845,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -1034,7 +1058,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1042,17 +1066,17 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1066,12 +1090,12 @@
   <dimension ref="A1:BJ70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="2"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="7" max="7" width="6.21875" customWidth="1"/>
@@ -1088,7 +1112,7 @@
         <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>0</v>
@@ -1121,16 +1145,16 @@
         <v>39</v>
       </c>
       <c r="AX1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BF1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.3">
@@ -1144,82 +1168,82 @@
         <v>45</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O2" t="s">
         <v>37</v>
       </c>
       <c r="P2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="S2" t="s">
         <v>37</v>
       </c>
       <c r="T2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="W2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="X2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Z2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AD2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AI2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AJ2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AL2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AM2" t="s">
         <v>18</v>
       </c>
       <c r="AN2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AQ2" t="s">
         <v>37</v>
       </c>
       <c r="AR2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AT2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AU2" t="s">
         <v>37</v>
       </c>
       <c r="AV2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.3">
@@ -1233,67 +1257,67 @@
         <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="O3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="R3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="S3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="W3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="X3" t="s">
         <v>21</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AI3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AJ3" t="s">
         <v>21</v>
       </c>
       <c r="AP3" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AQ3" t="s">
         <v>37</v>
       </c>
       <c r="AR3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AV3" t="s">
         <v>86</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>95</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.3">
@@ -1307,55 +1331,55 @@
         <v>23</v>
       </c>
       <c r="N4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="O4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P4" t="s">
         <v>21</v>
       </c>
       <c r="R4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T4" t="s">
         <v>21</v>
       </c>
       <c r="V4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="W4" t="s">
         <v>37</v>
       </c>
       <c r="X4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AH4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AI4" t="s">
         <v>37</v>
       </c>
       <c r="AJ4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AP4" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AQ4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AR4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AT4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AU4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AV4" t="s">
         <v>21</v>
@@ -1363,63 +1387,63 @@
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="V5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="W5" t="s">
         <v>37</v>
       </c>
       <c r="X5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AP5" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AQ5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AR5" t="s">
         <v>21</v>
       </c>
       <c r="AT5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AU5" t="s">
         <v>19</v>
       </c>
       <c r="AV5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>122</v>
       </c>
       <c r="AP6" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AQ6" t="s">
         <v>18</v>
       </c>
       <c r="AR6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AT6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AU6" t="s">
         <v>19</v>
@@ -1430,196 +1454,218 @@
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>124</v>
       </c>
       <c r="AP7" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AQ7" t="s">
         <v>18</v>
       </c>
       <c r="AR7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AT7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AU7" t="s">
         <v>18</v>
       </c>
       <c r="AV7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>64</v>
+        <v>125</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>18</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>66</v>
+      <c r="A20" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>67</v>
+      <c r="A21" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B22"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B23"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1629,7 +1675,9 @@
       <c r="B26"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B27"/>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28"/>

</xml_diff>

<commit_message>
Tweaking intro stuff - Phana and Chenchi
</commit_message>
<xml_diff>
--- a/[Si] Lair of Shadows/[CP] Lair of Shadows/Chars.xlsx
+++ b/[Si] Lair of Shadows/[CP] Lair of Shadows/Chars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Steam\Steam\steamapps\common\Stardew Valley\SiMods\[Si]\ShadowSanctuary\[Si] Lair of Shadows\[CP] Lair of Shadows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Steam\Steam\steamapps\common\Stardew Valley\SiMods\[Si]\.ShadowSanctuary\[Si] Lair of Shadows\[CP] Lair of Shadows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46FDDDD-3989-4854-AE74-2955D4AA2A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3FC3B5-AA58-411F-ABA2-3A72BEE76D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chars" sheetId="1" r:id="rId1"/>
@@ -786,11 +786,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -906,9 +906,7 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -1089,7 +1087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A12419-1E06-4537-9746-97A990338324}">
   <dimension ref="A1:BJ70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>